<commit_message>
Made Venn plots to see glm and sensory-motor electrode overlapped.
</commit_message>
<xml_diff>
--- a/projects/GLM/BNA_subregions.xlsx
+++ b/projects/GLM/BNA_subregions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bsliang_Coganlabcode\coganlab_ieeg\projects\GLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E11250F-F2CB-4ECE-99CD-E57DBB8E19B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8005AD-6B69-4227-9284-3513A6D44A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12852" yWindow="4620" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1778,14 +1778,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2069,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115:G115"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2099,10 +2099,10 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1" t="s">
         <v>529</v>
       </c>
@@ -2114,10 +2114,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2129,10 +2129,10 @@
       <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2141,8 +2141,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
@@ -2152,10 +2152,10 @@
       <c r="E3" s="3">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2164,8 +2164,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="E4" s="3">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2187,8 +2187,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2198,10 +2198,10 @@
       <c r="E5" s="3">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2210,8 +2210,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2221,10 +2221,10 @@
       <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2233,8 +2233,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
@@ -2244,10 +2244,10 @@
       <c r="E7" s="3">
         <v>12</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2" t="s">
         <v>29</v>
       </c>
@@ -2256,8 +2256,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
@@ -2267,10 +2267,10 @@
       <c r="E8" s="3">
         <v>14</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="2" t="s">
         <v>33</v>
       </c>
@@ -2279,8 +2279,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2292,10 +2292,10 @@
       <c r="E9" s="3">
         <v>16</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2304,8 +2304,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2315,10 +2315,10 @@
       <c r="E10" s="3">
         <v>18</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="2" t="s">
         <v>42</v>
       </c>
@@ -2327,8 +2327,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
@@ -2338,10 +2338,10 @@
       <c r="E11" s="3">
         <v>20</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2350,8 +2350,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
@@ -2361,10 +2361,10 @@
       <c r="E12" s="3">
         <v>22</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="2" t="s">
         <v>50</v>
       </c>
@@ -2373,8 +2373,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
@@ -2384,10 +2384,10 @@
       <c r="E13" s="3">
         <v>24</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="2" t="s">
         <v>54</v>
       </c>
@@ -2396,8 +2396,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
@@ -2407,10 +2407,10 @@
       <c r="E14" s="3">
         <v>26</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="2" t="s">
         <v>58</v>
       </c>
@@ -2419,8 +2419,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
         <v>60</v>
       </c>
@@ -2430,10 +2430,10 @@
       <c r="E15" s="3">
         <v>28</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="2" t="s">
         <v>62</v>
       </c>
@@ -2442,8 +2442,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2455,10 +2455,10 @@
       <c r="E16" s="3">
         <v>30</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="2" t="s">
         <v>67</v>
       </c>
@@ -2467,8 +2467,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="3" t="s">
         <v>69</v>
       </c>
@@ -2478,10 +2478,10 @@
       <c r="E17" s="3">
         <v>32</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="2" t="s">
         <v>71</v>
       </c>
@@ -2490,8 +2490,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="3" t="s">
         <v>73</v>
       </c>
@@ -2501,10 +2501,10 @@
       <c r="E18" s="3">
         <v>34</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="2" t="s">
         <v>75</v>
       </c>
@@ -2513,8 +2513,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="3" t="s">
         <v>77</v>
       </c>
@@ -2524,10 +2524,10 @@
       <c r="E19" s="3">
         <v>36</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="2" t="s">
         <v>79</v>
       </c>
@@ -2536,8 +2536,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="3" t="s">
         <v>81</v>
       </c>
@@ -2547,10 +2547,10 @@
       <c r="E20" s="3">
         <v>38</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="2" t="s">
         <v>83</v>
       </c>
@@ -2559,8 +2559,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="3" t="s">
         <v>85</v>
       </c>
@@ -2570,10 +2570,10 @@
       <c r="E21" s="3">
         <v>40</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="2" t="s">
         <v>87</v>
       </c>
@@ -2582,8 +2582,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -2595,10 +2595,10 @@
       <c r="E22" s="3">
         <v>42</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="2" t="s">
         <v>92</v>
       </c>
@@ -2607,8 +2607,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="3" t="s">
         <v>94</v>
       </c>
@@ -2618,10 +2618,10 @@
       <c r="E23" s="3">
         <v>44</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="2" t="s">
         <v>96</v>
       </c>
@@ -2630,8 +2630,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="3" t="s">
         <v>98</v>
       </c>
@@ -2641,10 +2641,10 @@
       <c r="E24" s="3">
         <v>46</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="2" t="s">
         <v>100</v>
       </c>
@@ -2653,8 +2653,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="3" t="s">
         <v>102</v>
       </c>
@@ -2664,10 +2664,10 @@
       <c r="E25" s="3">
         <v>48</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="2" t="s">
         <v>104</v>
       </c>
@@ -2676,8 +2676,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="3" t="s">
         <v>106</v>
       </c>
@@ -2687,10 +2687,10 @@
       <c r="E26" s="3">
         <v>50</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="2" t="s">
         <v>108</v>
       </c>
@@ -2699,8 +2699,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="3" t="s">
         <v>110</v>
       </c>
@@ -2710,10 +2710,10 @@
       <c r="E27" s="3">
         <v>52</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="5"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="2" t="s">
         <v>112</v>
       </c>
@@ -2722,8 +2722,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2735,10 +2735,10 @@
       <c r="E28" s="3">
         <v>54</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="2" t="s">
         <v>117</v>
       </c>
@@ -2747,8 +2747,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="3" t="s">
         <v>119</v>
       </c>
@@ -2758,10 +2758,10 @@
       <c r="E29" s="3">
         <v>56</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="5"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="2" t="s">
         <v>121</v>
       </c>
@@ -2770,8 +2770,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="6"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="3" t="s">
         <v>123</v>
       </c>
@@ -2781,10 +2781,10 @@
       <c r="E30" s="3">
         <v>58</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G30" s="5"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="2" t="s">
         <v>125</v>
       </c>
@@ -2793,8 +2793,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="3" t="s">
         <v>127</v>
       </c>
@@ -2804,10 +2804,10 @@
       <c r="E31" s="3">
         <v>60</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G31" s="5"/>
+      <c r="G31" s="6"/>
       <c r="H31" s="2" t="s">
         <v>129</v>
       </c>
@@ -2816,8 +2816,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="3" t="s">
         <v>131</v>
       </c>
@@ -2827,10 +2827,10 @@
       <c r="E32" s="3">
         <v>62</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="2" t="s">
         <v>133</v>
       </c>
@@ -2839,8 +2839,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="3" t="s">
         <v>135</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="E33" s="3">
         <v>64</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="2" t="s">
         <v>137</v>
       </c>
@@ -2862,8 +2862,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -2875,10 +2875,10 @@
       <c r="E34" s="3">
         <v>66</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="G34" s="6"/>
       <c r="H34" s="2" t="s">
         <v>142</v>
       </c>
@@ -2887,8 +2887,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="3" t="s">
         <v>144</v>
       </c>
@@ -2898,10 +2898,10 @@
       <c r="E35" s="3">
         <v>68</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="2" t="s">
         <v>146</v>
       </c>
@@ -2910,10 +2910,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2925,10 +2925,10 @@
       <c r="E36" s="3">
         <v>70</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="G36" s="5"/>
+      <c r="G36" s="6"/>
       <c r="H36" s="2" t="s">
         <v>152</v>
       </c>
@@ -2937,8 +2937,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1">
-      <c r="A37" s="6"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="3" t="s">
         <v>154</v>
       </c>
@@ -2948,10 +2948,10 @@
       <c r="E37" s="3">
         <v>72</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G37" s="5"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="2" t="s">
         <v>156</v>
       </c>
@@ -2960,8 +2960,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1">
-      <c r="A38" s="6"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="3" t="s">
         <v>158</v>
       </c>
@@ -2971,10 +2971,10 @@
       <c r="E38" s="3">
         <v>74</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="2" t="s">
         <v>160</v>
       </c>
@@ -2983,8 +2983,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1">
-      <c r="A39" s="6"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="3" t="s">
         <v>162</v>
       </c>
@@ -2994,10 +2994,10 @@
       <c r="E39" s="3">
         <v>76</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G39" s="5"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="2" t="s">
         <v>164</v>
       </c>
@@ -3006,8 +3006,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1">
-      <c r="A40" s="6"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="3" t="s">
         <v>166</v>
       </c>
@@ -3017,10 +3017,10 @@
       <c r="E40" s="3">
         <v>78</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="G40" s="5"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="2" t="s">
         <v>168</v>
       </c>
@@ -3029,8 +3029,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="18" customHeight="1">
-      <c r="A41" s="6"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="3" t="s">
         <v>170</v>
       </c>
@@ -3040,10 +3040,10 @@
       <c r="E41" s="3">
         <v>80</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="G41" s="5"/>
+      <c r="G41" s="6"/>
       <c r="H41" s="2" t="s">
         <v>172</v>
       </c>
@@ -3052,8 +3052,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1">
-      <c r="A42" s="6"/>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5" t="s">
         <v>174</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -3065,10 +3065,10 @@
       <c r="E42" s="3">
         <v>82</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G42" s="5"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="2" t="s">
         <v>177</v>
       </c>
@@ -3077,8 +3077,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" customHeight="1">
-      <c r="A43" s="6"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="3" t="s">
         <v>179</v>
       </c>
@@ -3088,10 +3088,10 @@
       <c r="E43" s="3">
         <v>84</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="2" t="s">
         <v>181</v>
       </c>
@@ -3100,8 +3100,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="18" customHeight="1">
-      <c r="A44" s="6"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="3" t="s">
         <v>183</v>
       </c>
@@ -3111,10 +3111,10 @@
       <c r="E44" s="3">
         <v>86</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G44" s="5"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="2" t="s">
         <v>185</v>
       </c>
@@ -3123,8 +3123,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="18" customHeight="1">
-      <c r="A45" s="6"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="3" t="s">
         <v>187</v>
       </c>
@@ -3134,10 +3134,10 @@
       <c r="E45" s="3">
         <v>88</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="G45" s="6"/>
       <c r="H45" s="2" t="s">
         <v>189</v>
       </c>
@@ -3146,8 +3146,8 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="18" customHeight="1">
-      <c r="A46" s="6"/>
-      <c r="B46" s="4" t="s">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5" t="s">
         <v>191</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -3159,10 +3159,10 @@
       <c r="E46" s="3">
         <v>90</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="G46" s="5"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="2" t="s">
         <v>194</v>
       </c>
@@ -3171,8 +3171,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="18" customHeight="1">
-      <c r="A47" s="6"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="3" t="s">
         <v>196</v>
       </c>
@@ -3182,10 +3182,10 @@
       <c r="E47" s="3">
         <v>92</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G47" s="5"/>
+      <c r="G47" s="6"/>
       <c r="H47" s="2" t="s">
         <v>198</v>
       </c>
@@ -3194,8 +3194,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="18" customHeight="1">
-      <c r="A48" s="6"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="3" t="s">
         <v>200</v>
       </c>
@@ -3205,10 +3205,10 @@
       <c r="E48" s="3">
         <v>94</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G48" s="5"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="2" t="s">
         <v>202</v>
       </c>
@@ -3217,8 +3217,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="18" customHeight="1">
-      <c r="A49" s="6"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
       <c r="C49" s="3" t="s">
         <v>204</v>
       </c>
@@ -3228,10 +3228,10 @@
       <c r="E49" s="3">
         <v>96</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G49" s="5"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="2" t="s">
         <v>206</v>
       </c>
@@ -3240,8 +3240,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="18" customHeight="1">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="3" t="s">
         <v>208</v>
       </c>
@@ -3251,10 +3251,10 @@
       <c r="E50" s="3">
         <v>98</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="G50" s="5"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="2" t="s">
         <v>210</v>
       </c>
@@ -3263,8 +3263,8 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="18" customHeight="1">
-      <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="3" t="s">
         <v>212</v>
       </c>
@@ -3274,10 +3274,10 @@
       <c r="E51" s="3">
         <v>100</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G51" s="5"/>
+      <c r="G51" s="6"/>
       <c r="H51" s="2" t="s">
         <v>214</v>
       </c>
@@ -3286,8 +3286,8 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="18" customHeight="1">
-      <c r="A52" s="6"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
       <c r="C52" s="3" t="s">
         <v>216</v>
       </c>
@@ -3297,10 +3297,10 @@
       <c r="E52" s="3">
         <v>102</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="G52" s="5"/>
+      <c r="G52" s="6"/>
       <c r="H52" s="2" t="s">
         <v>218</v>
       </c>
@@ -3309,8 +3309,8 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="18" customHeight="1">
-      <c r="A53" s="6"/>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -3322,10 +3322,10 @@
       <c r="E53" s="3">
         <v>104</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="G53" s="5"/>
+      <c r="G53" s="6"/>
       <c r="H53" s="2" t="s">
         <v>223</v>
       </c>
@@ -3334,8 +3334,8 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="18" customHeight="1">
-      <c r="A54" s="6"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="3" t="s">
         <v>225</v>
       </c>
@@ -3345,10 +3345,10 @@
       <c r="E54" s="3">
         <v>106</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G54" s="5"/>
+      <c r="G54" s="6"/>
       <c r="H54" s="2" t="s">
         <v>227</v>
       </c>
@@ -3357,8 +3357,8 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="18" customHeight="1">
-      <c r="A55" s="6"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="3" t="s">
         <v>229</v>
       </c>
@@ -3368,10 +3368,10 @@
       <c r="E55" s="3">
         <v>108</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="G55" s="5"/>
+      <c r="G55" s="6"/>
       <c r="H55" s="2" t="s">
         <v>231</v>
       </c>
@@ -3380,8 +3380,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="18" customHeight="1">
-      <c r="A56" s="6"/>
-      <c r="B56" s="4" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5" t="s">
         <v>233</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3393,10 +3393,10 @@
       <c r="E56" s="3">
         <v>110</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="G56" s="5"/>
+      <c r="G56" s="6"/>
       <c r="H56" s="2" t="s">
         <v>236</v>
       </c>
@@ -3405,8 +3405,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" customHeight="1">
-      <c r="A57" s="6"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="3" t="s">
         <v>238</v>
       </c>
@@ -3416,10 +3416,10 @@
       <c r="E57" s="3">
         <v>112</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="G57" s="5"/>
+      <c r="G57" s="6"/>
       <c r="H57" s="2" t="s">
         <v>240</v>
       </c>
@@ -3428,8 +3428,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="18" customHeight="1">
-      <c r="A58" s="6"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
       <c r="C58" s="3" t="s">
         <v>242</v>
       </c>
@@ -3439,10 +3439,10 @@
       <c r="E58" s="3">
         <v>114</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G58" s="5"/>
+      <c r="G58" s="6"/>
       <c r="H58" s="2" t="s">
         <v>244</v>
       </c>
@@ -3451,8 +3451,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="18" customHeight="1">
-      <c r="A59" s="6"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
       <c r="C59" s="3" t="s">
         <v>246</v>
       </c>
@@ -3462,10 +3462,10 @@
       <c r="E59" s="3">
         <v>116</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G59" s="5"/>
+      <c r="G59" s="6"/>
       <c r="H59" s="2" t="s">
         <v>248</v>
       </c>
@@ -3474,8 +3474,8 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="18" customHeight="1">
-      <c r="A60" s="6"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
       <c r="C60" s="3" t="s">
         <v>250</v>
       </c>
@@ -3485,10 +3485,10 @@
       <c r="E60" s="3">
         <v>118</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="G60" s="5"/>
+      <c r="G60" s="6"/>
       <c r="H60" s="2" t="s">
         <v>252</v>
       </c>
@@ -3497,8 +3497,8 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="18" customHeight="1">
-      <c r="A61" s="6"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
       <c r="C61" s="3" t="s">
         <v>254</v>
       </c>
@@ -3508,10 +3508,10 @@
       <c r="E61" s="3">
         <v>120</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G61" s="5"/>
+      <c r="G61" s="6"/>
       <c r="H61" s="2" t="s">
         <v>256</v>
       </c>
@@ -3520,8 +3520,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" customHeight="1">
-      <c r="A62" s="6"/>
-      <c r="B62" s="4" t="s">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5" t="s">
         <v>258</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -3533,10 +3533,10 @@
       <c r="E62" s="3">
         <v>122</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="G62" s="5"/>
+      <c r="G62" s="6"/>
       <c r="H62" s="2" t="s">
         <v>261</v>
       </c>
@@ -3545,8 +3545,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="18" customHeight="1">
-      <c r="A63" s="6"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
       <c r="C63" s="3" t="s">
         <v>263</v>
       </c>
@@ -3556,10 +3556,10 @@
       <c r="E63" s="3">
         <v>124</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="G63" s="5"/>
+      <c r="G63" s="6"/>
       <c r="H63" s="2" t="s">
         <v>264</v>
       </c>
@@ -3568,10 +3568,10 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="18" customHeight="1">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5" t="s">
         <v>267</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -3583,10 +3583,10 @@
       <c r="E64" s="3">
         <v>126</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="G64" s="5"/>
+      <c r="G64" s="6"/>
       <c r="H64" s="2" t="s">
         <v>270</v>
       </c>
@@ -3595,8 +3595,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="6"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="5"/>
       <c r="C65" s="3" t="s">
         <v>272</v>
       </c>
@@ -3606,10 +3606,10 @@
       <c r="E65" s="3">
         <v>128</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="G65" s="5"/>
+      <c r="G65" s="6"/>
       <c r="H65" s="2" t="s">
         <v>274</v>
       </c>
@@ -3618,8 +3618,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="18" customHeight="1">
-      <c r="A66" s="6"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
       <c r="C66" s="3" t="s">
         <v>276</v>
       </c>
@@ -3629,10 +3629,10 @@
       <c r="E66" s="3">
         <v>130</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="G66" s="5"/>
+      <c r="G66" s="6"/>
       <c r="H66" s="2" t="s">
         <v>278</v>
       </c>
@@ -3641,8 +3641,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="6"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
       <c r="C67" s="3" t="s">
         <v>280</v>
       </c>
@@ -3652,10 +3652,10 @@
       <c r="E67" s="3">
         <v>132</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="G67" s="5"/>
+      <c r="G67" s="6"/>
       <c r="H67" s="2" t="s">
         <v>282</v>
       </c>
@@ -3664,8 +3664,8 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="6"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
       <c r="C68" s="3" t="s">
         <v>284</v>
       </c>
@@ -3675,10 +3675,10 @@
       <c r="E68" s="3">
         <v>134</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="G68" s="5"/>
+      <c r="G68" s="6"/>
       <c r="H68" s="2" t="s">
         <v>286</v>
       </c>
@@ -3687,8 +3687,8 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="6"/>
-      <c r="B69" s="4" t="s">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5" t="s">
         <v>288</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -3700,10 +3700,10 @@
       <c r="E69" s="3">
         <v>136</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="G69" s="5"/>
+      <c r="G69" s="6"/>
       <c r="H69" s="2" t="s">
         <v>291</v>
       </c>
@@ -3712,8 +3712,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="18" customHeight="1">
-      <c r="A70" s="6"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
       <c r="C70" s="3" t="s">
         <v>293</v>
       </c>
@@ -3723,10 +3723,10 @@
       <c r="E70" s="3">
         <v>138</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="G70" s="5"/>
+      <c r="G70" s="6"/>
       <c r="H70" s="2" t="s">
         <v>295</v>
       </c>
@@ -3735,8 +3735,8 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="18" customHeight="1">
-      <c r="A71" s="6"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="5"/>
       <c r="C71" s="3" t="s">
         <v>297</v>
       </c>
@@ -3746,10 +3746,10 @@
       <c r="E71" s="3">
         <v>140</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="G71" s="5"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="2" t="s">
         <v>299</v>
       </c>
@@ -3758,8 +3758,8 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="18" customHeight="1">
-      <c r="A72" s="6"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="5"/>
       <c r="C72" s="3" t="s">
         <v>301</v>
       </c>
@@ -3769,10 +3769,10 @@
       <c r="E72" s="3">
         <v>142</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="G72" s="5"/>
+      <c r="G72" s="6"/>
       <c r="H72" s="2" t="s">
         <v>303</v>
       </c>
@@ -3781,8 +3781,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="18" customHeight="1">
-      <c r="A73" s="6"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="5"/>
       <c r="C73" s="3" t="s">
         <v>305</v>
       </c>
@@ -3792,10 +3792,10 @@
       <c r="E73" s="3">
         <v>144</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="G73" s="5"/>
+      <c r="G73" s="6"/>
       <c r="H73" s="2" t="s">
         <v>307</v>
       </c>
@@ -3804,8 +3804,8 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="18" customHeight="1">
-      <c r="A74" s="6"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="5"/>
       <c r="C74" s="3" t="s">
         <v>309</v>
       </c>
@@ -3815,10 +3815,10 @@
       <c r="E74" s="3">
         <v>146</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="G74" s="5"/>
+      <c r="G74" s="6"/>
       <c r="H74" s="2" t="s">
         <v>311</v>
       </c>
@@ -3827,8 +3827,8 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="18" customHeight="1">
-      <c r="A75" s="6"/>
-      <c r="B75" s="4" t="s">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -3840,10 +3840,10 @@
       <c r="E75" s="3">
         <v>148</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="G75" s="5"/>
+      <c r="G75" s="6"/>
       <c r="H75" s="2" t="s">
         <v>316</v>
       </c>
@@ -3852,8 +3852,8 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="18" customHeight="1">
-      <c r="A76" s="6"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="5"/>
       <c r="C76" s="3" t="s">
         <v>318</v>
       </c>
@@ -3863,10 +3863,10 @@
       <c r="E76" s="3">
         <v>150</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="G76" s="5"/>
+      <c r="G76" s="6"/>
       <c r="H76" s="2" t="s">
         <v>320</v>
       </c>
@@ -3875,8 +3875,8 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="18" customHeight="1">
-      <c r="A77" s="6"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="5"/>
       <c r="C77" s="3" t="s">
         <v>322</v>
       </c>
@@ -3886,10 +3886,10 @@
       <c r="E77" s="3">
         <v>152</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="G77" s="5"/>
+      <c r="G77" s="6"/>
       <c r="H77" s="2" t="s">
         <v>324</v>
       </c>
@@ -3898,8 +3898,8 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="18" customHeight="1">
-      <c r="A78" s="6"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="5"/>
       <c r="C78" s="3" t="s">
         <v>326</v>
       </c>
@@ -3909,10 +3909,10 @@
       <c r="E78" s="3">
         <v>154</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="G78" s="5"/>
+      <c r="G78" s="6"/>
       <c r="H78" s="2" t="s">
         <v>328</v>
       </c>
@@ -3921,8 +3921,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="18" customHeight="1">
-      <c r="A79" s="6"/>
-      <c r="B79" s="4" t="s">
+      <c r="A79" s="4"/>
+      <c r="B79" s="5" t="s">
         <v>330</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -3934,10 +3934,10 @@
       <c r="E79" s="3">
         <v>156</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="G79" s="5"/>
+      <c r="G79" s="6"/>
       <c r="H79" s="2" t="s">
         <v>333</v>
       </c>
@@ -3946,8 +3946,8 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="18" customHeight="1">
-      <c r="A80" s="6"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="5"/>
       <c r="C80" s="3" t="s">
         <v>335</v>
       </c>
@@ -3957,10 +3957,10 @@
       <c r="E80" s="3">
         <v>158</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="G80" s="5"/>
+      <c r="G80" s="6"/>
       <c r="H80" s="2" t="s">
         <v>337</v>
       </c>
@@ -3969,8 +3969,8 @@
       </c>
     </row>
     <row r="81" spans="1:9" ht="18" customHeight="1">
-      <c r="A81" s="6"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
       <c r="C81" s="3" t="s">
         <v>339</v>
       </c>
@@ -3980,10 +3980,10 @@
       <c r="E81" s="3">
         <v>160</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="G81" s="5"/>
+      <c r="G81" s="6"/>
       <c r="H81" s="2" t="s">
         <v>341</v>
       </c>
@@ -3992,8 +3992,8 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" customHeight="1">
-      <c r="A82" s="6"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
       <c r="C82" s="3" t="s">
         <v>343</v>
       </c>
@@ -4003,10 +4003,10 @@
       <c r="E82" s="3">
         <v>162</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G82" s="5"/>
+      <c r="G82" s="6"/>
       <c r="H82" s="2" t="s">
         <v>345</v>
       </c>
@@ -4015,10 +4015,10 @@
       </c>
     </row>
     <row r="83" spans="1:9" ht="18" customHeight="1">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="5" t="s">
         <v>348</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -4030,10 +4030,10 @@
       <c r="E83" s="3">
         <v>164</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F83" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="G83" s="5"/>
+      <c r="G83" s="6"/>
       <c r="H83" s="2" t="s">
         <v>351</v>
       </c>
@@ -4042,8 +4042,8 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="18" customHeight="1">
-      <c r="A84" s="6"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="5"/>
       <c r="C84" s="3" t="s">
         <v>353</v>
       </c>
@@ -4053,10 +4053,10 @@
       <c r="E84" s="3">
         <v>166</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="G84" s="5"/>
+      <c r="G84" s="6"/>
       <c r="H84" s="2" t="s">
         <v>355</v>
       </c>
@@ -4065,8 +4065,8 @@
       </c>
     </row>
     <row r="85" spans="1:9" ht="18" customHeight="1">
-      <c r="A85" s="6"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="5"/>
       <c r="C85" s="3" t="s">
         <v>357</v>
       </c>
@@ -4076,10 +4076,10 @@
       <c r="E85" s="3">
         <v>168</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="G85" s="5"/>
+      <c r="G85" s="6"/>
       <c r="H85" s="2" t="s">
         <v>359</v>
       </c>
@@ -4088,8 +4088,8 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="18" customHeight="1">
-      <c r="A86" s="6"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="5"/>
       <c r="C86" s="3" t="s">
         <v>361</v>
       </c>
@@ -4099,10 +4099,10 @@
       <c r="E86" s="3">
         <v>170</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="G86" s="5"/>
+      <c r="G86" s="6"/>
       <c r="H86" s="2" t="s">
         <v>363</v>
       </c>
@@ -4111,8 +4111,8 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="18" customHeight="1">
-      <c r="A87" s="6"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="5"/>
       <c r="C87" s="3" t="s">
         <v>365</v>
       </c>
@@ -4122,10 +4122,10 @@
       <c r="E87" s="3">
         <v>172</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F87" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="G87" s="5"/>
+      <c r="G87" s="6"/>
       <c r="H87" s="2" t="s">
         <v>367</v>
       </c>
@@ -4134,8 +4134,8 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="18" customHeight="1">
-      <c r="A88" s="6"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="5"/>
       <c r="C88" s="3" t="s">
         <v>369</v>
       </c>
@@ -4145,10 +4145,10 @@
       <c r="E88" s="3">
         <v>174</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="G88" s="5"/>
+      <c r="G88" s="6"/>
       <c r="H88" s="2" t="s">
         <v>371</v>
       </c>
@@ -4157,10 +4157,10 @@
       </c>
     </row>
     <row r="89" spans="1:9" ht="18" customHeight="1">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="5" t="s">
         <v>374</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -4172,10 +4172,10 @@
       <c r="E89" s="3">
         <v>176</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F89" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="G89" s="5"/>
+      <c r="G89" s="6"/>
       <c r="H89" s="2" t="s">
         <v>377</v>
       </c>
@@ -4184,8 +4184,8 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="18" customHeight="1">
-      <c r="A90" s="6"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="5"/>
       <c r="C90" s="3" t="s">
         <v>379</v>
       </c>
@@ -4195,10 +4195,10 @@
       <c r="E90" s="3">
         <v>178</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="F90" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="G90" s="5"/>
+      <c r="G90" s="6"/>
       <c r="H90" s="2" t="s">
         <v>381</v>
       </c>
@@ -4207,8 +4207,8 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="18" customHeight="1">
-      <c r="A91" s="6"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="5"/>
       <c r="C91" s="3" t="s">
         <v>383</v>
       </c>
@@ -4218,10 +4218,10 @@
       <c r="E91" s="3">
         <v>180</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F91" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="G91" s="5"/>
+      <c r="G91" s="6"/>
       <c r="H91" s="2" t="s">
         <v>385</v>
       </c>
@@ -4230,8 +4230,8 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="18" customHeight="1">
-      <c r="A92" s="6"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="5"/>
       <c r="C92" s="3" t="s">
         <v>387</v>
       </c>
@@ -4241,10 +4241,10 @@
       <c r="E92" s="3">
         <v>182</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F92" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="G92" s="5"/>
+      <c r="G92" s="6"/>
       <c r="H92" s="2" t="s">
         <v>389</v>
       </c>
@@ -4253,8 +4253,8 @@
       </c>
     </row>
     <row r="93" spans="1:9" ht="18" customHeight="1">
-      <c r="A93" s="6"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="5"/>
       <c r="C93" s="3" t="s">
         <v>391</v>
       </c>
@@ -4264,10 +4264,10 @@
       <c r="E93" s="3">
         <v>184</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="F93" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="G93" s="5"/>
+      <c r="G93" s="6"/>
       <c r="H93" s="2" t="s">
         <v>393</v>
       </c>
@@ -4276,8 +4276,8 @@
       </c>
     </row>
     <row r="94" spans="1:9" ht="18" customHeight="1">
-      <c r="A94" s="6"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="5"/>
       <c r="C94" s="3" t="s">
         <v>395</v>
       </c>
@@ -4287,10 +4287,10 @@
       <c r="E94" s="3">
         <v>186</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F94" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G94" s="5"/>
+      <c r="G94" s="6"/>
       <c r="H94" s="2" t="s">
         <v>397</v>
       </c>
@@ -4299,8 +4299,8 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="18" customHeight="1">
-      <c r="A95" s="6"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="5"/>
       <c r="C95" s="3" t="s">
         <v>399</v>
       </c>
@@ -4310,10 +4310,10 @@
       <c r="E95" s="3">
         <v>188</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F95" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="G95" s="5"/>
+      <c r="G95" s="6"/>
       <c r="H95" s="2" t="s">
         <v>401</v>
       </c>
@@ -4322,10 +4322,10 @@
       </c>
     </row>
     <row r="96" spans="1:9" ht="18" customHeight="1">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="5" t="s">
         <v>526</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -4337,10 +4337,10 @@
       <c r="E96" s="3">
         <v>190</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F96" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="G96" s="5"/>
+      <c r="G96" s="6"/>
       <c r="H96" s="2" t="s">
         <v>406</v>
       </c>
@@ -4349,8 +4349,8 @@
       </c>
     </row>
     <row r="97" spans="1:9" ht="18" customHeight="1">
-      <c r="A97" s="6"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="5"/>
       <c r="C97" s="3" t="s">
         <v>408</v>
       </c>
@@ -4360,10 +4360,10 @@
       <c r="E97" s="3">
         <v>192</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F97" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="G97" s="5"/>
+      <c r="G97" s="6"/>
       <c r="H97" s="2" t="s">
         <v>410</v>
       </c>
@@ -4372,8 +4372,8 @@
       </c>
     </row>
     <row r="98" spans="1:9" ht="18" customHeight="1">
-      <c r="A98" s="6"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="5"/>
       <c r="C98" s="3" t="s">
         <v>412</v>
       </c>
@@ -4383,10 +4383,10 @@
       <c r="E98" s="3">
         <v>194</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F98" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="G98" s="5"/>
+      <c r="G98" s="6"/>
       <c r="H98" s="2" t="s">
         <v>414</v>
       </c>
@@ -4395,8 +4395,8 @@
       </c>
     </row>
     <row r="99" spans="1:9" ht="18" customHeight="1">
-      <c r="A99" s="6"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="5"/>
       <c r="C99" s="3" t="s">
         <v>416</v>
       </c>
@@ -4406,10 +4406,10 @@
       <c r="E99" s="3">
         <v>196</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="G99" s="5"/>
+      <c r="G99" s="6"/>
       <c r="H99" s="2" t="s">
         <v>418</v>
       </c>
@@ -4418,8 +4418,8 @@
       </c>
     </row>
     <row r="100" spans="1:9" ht="18" customHeight="1">
-      <c r="A100" s="6"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="5"/>
       <c r="C100" s="3" t="s">
         <v>420</v>
       </c>
@@ -4429,10 +4429,10 @@
       <c r="E100" s="3">
         <v>198</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F100" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="G100" s="5"/>
+      <c r="G100" s="6"/>
       <c r="H100" s="2" t="s">
         <v>422</v>
       </c>
@@ -4441,8 +4441,8 @@
       </c>
     </row>
     <row r="101" spans="1:9" ht="18" customHeight="1">
-      <c r="A101" s="6"/>
-      <c r="B101" s="4" t="s">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5" t="s">
         <v>424</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -4454,10 +4454,10 @@
       <c r="E101" s="3">
         <v>200</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F101" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="G101" s="5"/>
+      <c r="G101" s="6"/>
       <c r="H101" s="2" t="s">
         <v>427</v>
       </c>
@@ -4466,8 +4466,8 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="18" customHeight="1">
-      <c r="A102" s="6"/>
-      <c r="B102" s="4"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="5"/>
       <c r="C102" s="3" t="s">
         <v>429</v>
       </c>
@@ -4477,10 +4477,10 @@
       <c r="E102" s="3">
         <v>202</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="G102" s="5"/>
+      <c r="G102" s="6"/>
       <c r="H102" s="2" t="s">
         <v>431</v>
       </c>
@@ -4489,8 +4489,8 @@
       </c>
     </row>
     <row r="103" spans="1:9" ht="18" customHeight="1">
-      <c r="A103" s="6"/>
-      <c r="B103" s="4"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="5"/>
       <c r="C103" s="3" t="s">
         <v>433</v>
       </c>
@@ -4500,10 +4500,10 @@
       <c r="E103" s="3">
         <v>204</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F103" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="G103" s="5"/>
+      <c r="G103" s="6"/>
       <c r="H103" s="2" t="s">
         <v>435</v>
       </c>
@@ -4512,8 +4512,8 @@
       </c>
     </row>
     <row r="104" spans="1:9" ht="18" customHeight="1">
-      <c r="A104" s="6"/>
-      <c r="B104" s="4"/>
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
       <c r="C104" s="3" t="s">
         <v>437</v>
       </c>
@@ -4523,10 +4523,10 @@
       <c r="E104" s="3">
         <v>206</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="F104" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="G104" s="5"/>
+      <c r="G104" s="6"/>
       <c r="H104" s="2" t="s">
         <v>439</v>
       </c>
@@ -4535,8 +4535,8 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="18" customHeight="1">
-      <c r="A105" s="6"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="5"/>
       <c r="C105" s="3" t="s">
         <v>441</v>
       </c>
@@ -4546,10 +4546,10 @@
       <c r="E105" s="3">
         <v>208</v>
       </c>
-      <c r="F105" s="5" t="s">
+      <c r="F105" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="G105" s="5"/>
+      <c r="G105" s="6"/>
       <c r="H105" s="2" t="s">
         <v>443</v>
       </c>
@@ -4558,8 +4558,8 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="18" customHeight="1">
-      <c r="A106" s="6"/>
-      <c r="B106" s="4"/>
+      <c r="A106" s="4"/>
+      <c r="B106" s="5"/>
       <c r="C106" s="3" t="s">
         <v>445</v>
       </c>
@@ -4569,10 +4569,10 @@
       <c r="E106" s="3">
         <v>210</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="F106" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="G106" s="5"/>
+      <c r="G106" s="6"/>
       <c r="H106" s="2" t="s">
         <v>447</v>
       </c>
@@ -4581,10 +4581,10 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="18" customHeight="1">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="5" t="s">
         <v>450</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -4596,10 +4596,10 @@
       <c r="E107" s="3">
         <v>212</v>
       </c>
-      <c r="F107" s="5" t="s">
+      <c r="F107" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="G107" s="5"/>
+      <c r="G107" s="6"/>
       <c r="H107" s="2" t="s">
         <v>453</v>
       </c>
@@ -4608,8 +4608,8 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="18" customHeight="1">
-      <c r="A108" s="6"/>
-      <c r="B108" s="4"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="5"/>
       <c r="C108" s="3" t="s">
         <v>455</v>
       </c>
@@ -4619,10 +4619,10 @@
       <c r="E108" s="3">
         <v>214</v>
       </c>
-      <c r="F108" s="5" t="s">
+      <c r="F108" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="G108" s="5"/>
+      <c r="G108" s="6"/>
       <c r="H108" s="2" t="s">
         <v>457</v>
       </c>
@@ -4631,8 +4631,8 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="18" customHeight="1">
-      <c r="A109" s="6"/>
-      <c r="B109" s="4" t="s">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5" t="s">
         <v>459</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -4644,10 +4644,10 @@
       <c r="E109" s="3">
         <v>216</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="F109" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="G109" s="5"/>
+      <c r="G109" s="6"/>
       <c r="H109" s="2" t="s">
         <v>462</v>
       </c>
@@ -4656,8 +4656,8 @@
       </c>
     </row>
     <row r="110" spans="1:9" ht="18" customHeight="1">
-      <c r="A110" s="6"/>
-      <c r="B110" s="4"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="5"/>
       <c r="C110" s="3" t="s">
         <v>464</v>
       </c>
@@ -4667,10 +4667,10 @@
       <c r="E110" s="3">
         <v>218</v>
       </c>
-      <c r="F110" s="5" t="s">
+      <c r="F110" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="G110" s="5"/>
+      <c r="G110" s="6"/>
       <c r="H110" s="2" t="s">
         <v>466</v>
       </c>
@@ -4679,8 +4679,8 @@
       </c>
     </row>
     <row r="111" spans="1:9" ht="18" customHeight="1">
-      <c r="A111" s="6"/>
-      <c r="B111" s="4" t="s">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5" t="s">
         <v>468</v>
       </c>
       <c r="C111" s="3" t="s">
@@ -4692,10 +4692,10 @@
       <c r="E111" s="3">
         <v>220</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="F111" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G111" s="5"/>
+      <c r="G111" s="6"/>
       <c r="H111" s="2" t="s">
         <v>471</v>
       </c>
@@ -4704,8 +4704,8 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="18" customHeight="1">
-      <c r="A112" s="6"/>
-      <c r="B112" s="4"/>
+      <c r="A112" s="4"/>
+      <c r="B112" s="5"/>
       <c r="C112" s="3" t="s">
         <v>473</v>
       </c>
@@ -4715,10 +4715,10 @@
       <c r="E112" s="3">
         <v>222</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="F112" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="G112" s="5"/>
+      <c r="G112" s="6"/>
       <c r="H112" s="2" t="s">
         <v>475</v>
       </c>
@@ -4727,8 +4727,8 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="18" customHeight="1">
-      <c r="A113" s="6"/>
-      <c r="B113" s="4"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="5"/>
       <c r="C113" s="3" t="s">
         <v>477</v>
       </c>
@@ -4738,10 +4738,10 @@
       <c r="E113" s="3">
         <v>224</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F113" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="G113" s="5"/>
+      <c r="G113" s="6"/>
       <c r="H113" s="2" t="s">
         <v>479</v>
       </c>
@@ -4750,8 +4750,8 @@
       </c>
     </row>
     <row r="114" spans="1:9" ht="18" customHeight="1">
-      <c r="A114" s="6"/>
-      <c r="B114" s="4"/>
+      <c r="A114" s="4"/>
+      <c r="B114" s="5"/>
       <c r="C114" s="3" t="s">
         <v>481</v>
       </c>
@@ -4761,10 +4761,10 @@
       <c r="E114" s="3">
         <v>226</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F114" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="G114" s="5"/>
+      <c r="G114" s="6"/>
       <c r="H114" s="2" t="s">
         <v>483</v>
       </c>
@@ -4773,8 +4773,8 @@
       </c>
     </row>
     <row r="115" spans="1:9" ht="18" customHeight="1">
-      <c r="A115" s="6"/>
-      <c r="B115" s="4"/>
+      <c r="A115" s="4"/>
+      <c r="B115" s="5"/>
       <c r="C115" s="3" t="s">
         <v>485</v>
       </c>
@@ -4784,10 +4784,10 @@
       <c r="E115" s="3">
         <v>228</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F115" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="G115" s="5"/>
+      <c r="G115" s="6"/>
       <c r="H115" s="2" t="s">
         <v>487</v>
       </c>
@@ -4796,8 +4796,8 @@
       </c>
     </row>
     <row r="116" spans="1:9" ht="18" customHeight="1">
-      <c r="A116" s="6"/>
-      <c r="B116" s="4"/>
+      <c r="A116" s="4"/>
+      <c r="B116" s="5"/>
       <c r="C116" s="3" t="s">
         <v>489</v>
       </c>
@@ -4807,10 +4807,10 @@
       <c r="E116" s="3">
         <v>230</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F116" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="G116" s="5"/>
+      <c r="G116" s="6"/>
       <c r="H116" s="2" t="s">
         <v>491</v>
       </c>
@@ -4819,8 +4819,8 @@
       </c>
     </row>
     <row r="117" spans="1:9" ht="18" customHeight="1">
-      <c r="A117" s="6"/>
-      <c r="B117" s="4" t="s">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5" t="s">
         <v>493</v>
       </c>
       <c r="C117" s="3" t="s">
@@ -4832,10 +4832,10 @@
       <c r="E117" s="3">
         <v>232</v>
       </c>
-      <c r="F117" s="5" t="s">
+      <c r="F117" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="G117" s="5"/>
+      <c r="G117" s="6"/>
       <c r="H117" s="2" t="s">
         <v>496</v>
       </c>
@@ -4844,8 +4844,8 @@
       </c>
     </row>
     <row r="118" spans="1:9" ht="18" customHeight="1">
-      <c r="A118" s="6"/>
-      <c r="B118" s="4"/>
+      <c r="A118" s="4"/>
+      <c r="B118" s="5"/>
       <c r="C118" s="3" t="s">
         <v>498</v>
       </c>
@@ -4855,10 +4855,10 @@
       <c r="E118" s="3">
         <v>234</v>
       </c>
-      <c r="F118" s="5" t="s">
+      <c r="F118" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="G118" s="5"/>
+      <c r="G118" s="6"/>
       <c r="H118" s="2" t="s">
         <v>500</v>
       </c>
@@ -4867,8 +4867,8 @@
       </c>
     </row>
     <row r="119" spans="1:9" ht="18" customHeight="1">
-      <c r="A119" s="6"/>
-      <c r="B119" s="4"/>
+      <c r="A119" s="4"/>
+      <c r="B119" s="5"/>
       <c r="C119" s="3" t="s">
         <v>502</v>
       </c>
@@ -4878,10 +4878,10 @@
       <c r="E119" s="3">
         <v>236</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F119" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="G119" s="5"/>
+      <c r="G119" s="6"/>
       <c r="H119" s="2" t="s">
         <v>504</v>
       </c>
@@ -4890,8 +4890,8 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="18" customHeight="1">
-      <c r="A120" s="6"/>
-      <c r="B120" s="4"/>
+      <c r="A120" s="4"/>
+      <c r="B120" s="5"/>
       <c r="C120" s="3" t="s">
         <v>506</v>
       </c>
@@ -4901,10 +4901,10 @@
       <c r="E120" s="3">
         <v>238</v>
       </c>
-      <c r="F120" s="5" t="s">
+      <c r="F120" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G120" s="5"/>
+      <c r="G120" s="6"/>
       <c r="H120" s="2" t="s">
         <v>508</v>
       </c>
@@ -4913,8 +4913,8 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="18" customHeight="1">
-      <c r="A121" s="6"/>
-      <c r="B121" s="4"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="5"/>
       <c r="C121" s="3" t="s">
         <v>510</v>
       </c>
@@ -4924,10 +4924,10 @@
       <c r="E121" s="3">
         <v>240</v>
       </c>
-      <c r="F121" s="5" t="s">
+      <c r="F121" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="G121" s="5"/>
+      <c r="G121" s="6"/>
       <c r="H121" s="2" t="s">
         <v>512</v>
       </c>
@@ -4936,8 +4936,8 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="18" customHeight="1">
-      <c r="A122" s="6"/>
-      <c r="B122" s="4"/>
+      <c r="A122" s="4"/>
+      <c r="B122" s="5"/>
       <c r="C122" s="3" t="s">
         <v>514</v>
       </c>
@@ -4947,10 +4947,10 @@
       <c r="E122" s="3">
         <v>242</v>
       </c>
-      <c r="F122" s="5" t="s">
+      <c r="F122" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="G122" s="5"/>
+      <c r="G122" s="6"/>
       <c r="H122" s="2" t="s">
         <v>516</v>
       </c>
@@ -4959,8 +4959,8 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="18" customHeight="1">
-      <c r="A123" s="6"/>
-      <c r="B123" s="4"/>
+      <c r="A123" s="4"/>
+      <c r="B123" s="5"/>
       <c r="C123" s="3" t="s">
         <v>518</v>
       </c>
@@ -4970,10 +4970,10 @@
       <c r="E123" s="3">
         <v>244</v>
       </c>
-      <c r="F123" s="5" t="s">
+      <c r="F123" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="G123" s="5"/>
+      <c r="G123" s="6"/>
       <c r="H123" s="2" t="s">
         <v>520</v>
       </c>
@@ -4982,8 +4982,8 @@
       </c>
     </row>
     <row r="124" spans="1:9" ht="18" customHeight="1">
-      <c r="A124" s="6"/>
-      <c r="B124" s="4"/>
+      <c r="A124" s="4"/>
+      <c r="B124" s="5"/>
       <c r="C124" s="3" t="s">
         <v>522</v>
       </c>
@@ -4993,10 +4993,10 @@
       <c r="E124" s="3">
         <v>246</v>
       </c>
-      <c r="F124" s="5" t="s">
+      <c r="F124" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="G124" s="5"/>
+      <c r="G124" s="6"/>
       <c r="H124" s="2" t="s">
         <v>524</v>
       </c>
@@ -5006,6 +5006,137 @@
     </row>
   </sheetData>
   <mergeCells count="155">
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="F104:G104"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="B117:B124"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="F119:G119"/>
+    <mergeCell ref="F120:G120"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="A107:A124"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="F107:G107"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="A96:A106"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="B101:B106"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="B111:B116"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="F112:G112"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="A89:A95"/>
+    <mergeCell ref="B89:B95"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="F93:G93"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="A83:A88"/>
+    <mergeCell ref="B83:B88"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A64:A82"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:A63"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A2:A35"/>
     <mergeCell ref="B2:B8"/>
@@ -5030,137 +5161,6 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:A63"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="B69:B74"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A83:A88"/>
-    <mergeCell ref="B83:B88"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A64:A82"/>
-    <mergeCell ref="A89:A95"/>
-    <mergeCell ref="B89:B95"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="F93:G93"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="A107:A124"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="F107:G107"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="A96:A106"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="F97:G97"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="B101:B106"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="F110:G110"/>
-    <mergeCell ref="B111:B116"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="F112:G112"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="F104:G104"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="B117:B124"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F118:G118"/>
-    <mergeCell ref="F119:G119"/>
-    <mergeCell ref="F120:G120"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="F122:G122"/>
-    <mergeCell ref="F123:G123"/>
-    <mergeCell ref="F124:G124"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>